<commit_message>
corrected a link and erased column
</commit_message>
<xml_diff>
--- a/partlist.xlsx
+++ b/partlist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thilo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\01_Meine Dateien\03_Studium\02_Master\01_Semesterordner\04_4. Semester (SoSe16)\01_Digitale Messtechnik mit Mikrorechnern\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
   <si>
     <t>Bestellnr</t>
   </si>
@@ -35,12 +35,6 @@
     <t>Anzahl</t>
   </si>
   <si>
-    <t>Preis in €</t>
-  </si>
-  <si>
-    <t>Preis/Stck.</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
@@ -71,9 +65,6 @@
     <t>HF-/Koaxialsteckverbinder 50Ohm</t>
   </si>
   <si>
-    <t>de.farnell.com/multicomp/1712350/buchse-bnc-pcb-r-a-bulk/dp/2069808</t>
-  </si>
-  <si>
     <t>Chipwiderstand 100R</t>
   </si>
   <si>
@@ -417,6 +408,12 @@
   </si>
   <si>
     <t>1287414</t>
+  </si>
+  <si>
+    <t>http://de.farnell.com/multicomp/13-60-2-dgz/buchse-bnc-right-angle/dp/1712350</t>
+  </si>
+  <si>
+    <t>Preis/Stck. [€]</t>
   </si>
 </sst>
 </file>
@@ -771,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,12 +779,11 @@
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="100.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="100.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -798,21 +794,18 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2356154</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -820,39 +813,33 @@
       <c r="D2">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E2">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>7992033</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3">
-        <v>5.5</v>
-      </c>
-      <c r="E3">
         <v>2.75</v>
       </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2364018</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -860,319 +847,271 @@
       <c r="D4">
         <v>1.1499999999999999</v>
       </c>
-      <c r="E4">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2141505</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
-      </c>
-      <c r="C5">
-        <v>10</v>
-      </c>
-      <c r="D5">
-        <v>1.1999999999999999E-2</v>
-      </c>
-      <c r="E5">
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6">
-        <v>1.81</v>
-      </c>
-      <c r="E6">
-        <v>0.90500000000000003</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.98</v>
+      </c>
+      <c r="E6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>11</v>
       </c>
       <c r="D7">
-        <v>1.3199999999999998E-2</v>
-      </c>
-      <c r="E7">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2447226</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>10</v>
       </c>
       <c r="D8">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="E8">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>12</v>
       </c>
       <c r="D9">
-        <v>9.4800000000000009E-2</v>
-      </c>
-      <c r="E9">
         <v>7.9000000000000008E-3</v>
       </c>
-      <c r="F9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>19</v>
       </c>
       <c r="D10">
-        <v>6.6500000000000004E-2</v>
-      </c>
-      <c r="E10">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="F10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1703794</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11">
-        <v>3.48</v>
-      </c>
-      <c r="E11">
         <v>1.74</v>
       </c>
-      <c r="F11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9451056</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
       <c r="D12">
-        <v>0.17319999999999999</v>
-      </c>
-      <c r="E12">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="F12" t="s">
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>1.5E-3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="E14" t="s">
         <v>28</v>
       </c>
-      <c r="C13">
-        <v>10</v>
-      </c>
-      <c r="D13">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="E13">
-        <v>1.5E-3</v>
-      </c>
-      <c r="F13" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="E15" t="s">
         <v>30</v>
       </c>
-      <c r="C14">
-        <v>10</v>
-      </c>
-      <c r="D14">
-        <v>7.400000000000001E-2</v>
-      </c>
-      <c r="E14">
-        <v>7.4000000000000003E-3</v>
-      </c>
-      <c r="F14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15">
-        <v>10</v>
-      </c>
-      <c r="D15">
-        <v>1.1999999999999999E-2</v>
-      </c>
-      <c r="E15">
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="F15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1651089</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
       <c r="D16">
-        <v>0.20799999999999999</v>
-      </c>
-      <c r="E16">
         <v>0.104</v>
       </c>
-      <c r="F16" t="s">
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>1.5699999999999999E-2</v>
+      </c>
+      <c r="E18" t="s">
         <v>36</v>
       </c>
-      <c r="C17">
-        <v>10</v>
-      </c>
-      <c r="D17">
-        <v>0.14200000000000002</v>
-      </c>
-      <c r="E17">
-        <v>1.4200000000000001E-2</v>
-      </c>
-      <c r="F17" t="s">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18">
-        <v>10</v>
-      </c>
-      <c r="D18">
-        <v>0.15699999999999997</v>
-      </c>
-      <c r="E18">
-        <v>1.5699999999999999E-2</v>
-      </c>
-      <c r="F18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B19" t="s">
-        <v>40</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
       <c r="D19">
-        <v>0.1176</v>
-      </c>
-      <c r="E19">
         <v>5.8799999999999998E-2</v>
       </c>
-      <c r="F19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1180,99 +1119,84 @@
       <c r="D20">
         <v>0.14699999999999999</v>
       </c>
-      <c r="E20">
-        <v>0.14699999999999999</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="E20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21">
-        <v>10</v>
-      </c>
-      <c r="D21">
-        <v>1.1999999999999999E-2</v>
-      </c>
-      <c r="E21">
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="F21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B22" t="s">
-        <v>46</v>
       </c>
       <c r="C22">
         <v>11</v>
       </c>
       <c r="D22">
-        <v>0.6512</v>
-      </c>
-      <c r="E22">
         <v>5.9200000000000003E-2</v>
       </c>
-      <c r="F22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C23">
         <v>10</v>
       </c>
       <c r="D23">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="E23">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="F23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1170868</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C24">
         <v>10</v>
       </c>
       <c r="D24">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="E24">
         <v>1.5E-3</v>
       </c>
-      <c r="F24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1280,19 +1204,16 @@
       <c r="D25">
         <v>0.52900000000000003</v>
       </c>
-      <c r="E25">
-        <v>0.52900000000000003</v>
-      </c>
-      <c r="F25" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1300,19 +1221,16 @@
       <c r="D26">
         <v>0.51700000000000002</v>
       </c>
-      <c r="E26">
-        <v>0.51700000000000002</v>
-      </c>
-      <c r="F26" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1320,19 +1238,16 @@
       <c r="D27">
         <v>0.38700000000000001</v>
       </c>
-      <c r="E27">
-        <v>0.38700000000000001</v>
-      </c>
-      <c r="F27" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1340,39 +1255,33 @@
       <c r="D28">
         <v>0.438</v>
       </c>
-      <c r="E28">
-        <v>0.438</v>
-      </c>
-      <c r="F28" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C29">
         <v>2</v>
       </c>
       <c r="D29">
-        <v>0.76</v>
-      </c>
-      <c r="E29">
         <v>0.38</v>
       </c>
-      <c r="F29" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1380,139 +1289,118 @@
       <c r="D30">
         <v>0.35199999999999998</v>
       </c>
-      <c r="E30">
-        <v>0.35199999999999998</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="E30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31">
-        <v>10</v>
-      </c>
-      <c r="D31">
-        <v>4.7999999999999994E-2</v>
-      </c>
-      <c r="E31">
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="E34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <v>1.5E-3</v>
+      </c>
+      <c r="E35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36">
+        <v>10</v>
+      </c>
+      <c r="D36">
         <v>4.7999999999999996E-3</v>
       </c>
-      <c r="F31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B32" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32">
-        <v>10</v>
-      </c>
-      <c r="D32">
-        <v>1.6E-2</v>
-      </c>
-      <c r="E32">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="F32" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B33" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33">
-        <v>10</v>
-      </c>
-      <c r="D33">
-        <v>1.6E-2</v>
-      </c>
-      <c r="E33">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="F33" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="E36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B34" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34">
-        <v>10</v>
-      </c>
-      <c r="D34">
-        <v>1.6E-2</v>
-      </c>
-      <c r="E34">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="F34" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35">
-        <v>10</v>
-      </c>
-      <c r="D35">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="E35">
-        <v>1.5E-3</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="B37" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B36" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36">
-        <v>10</v>
-      </c>
-      <c r="D36">
-        <v>4.7999999999999994E-2</v>
-      </c>
-      <c r="E36">
-        <v>4.7999999999999996E-3</v>
-      </c>
-      <c r="F36" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B37" t="s">
-        <v>76</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -1520,19 +1408,16 @@
       <c r="D37">
         <v>2.57</v>
       </c>
-      <c r="E37">
-        <v>2.57</v>
-      </c>
-      <c r="F37" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>1607239</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -1540,59 +1425,50 @@
       <c r="D38">
         <v>2.52</v>
       </c>
-      <c r="E38">
-        <v>2.52</v>
-      </c>
-      <c r="F38" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C39">
         <v>5</v>
       </c>
       <c r="D39">
-        <v>0.14500000000000002</v>
-      </c>
-      <c r="E39">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="F39" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>1798068</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C40">
         <v>5</v>
       </c>
       <c r="D40">
-        <v>0.3705</v>
-      </c>
-      <c r="E40">
         <v>7.4099999999999999E-2</v>
       </c>
-      <c r="F40" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>497332</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -1600,39 +1476,33 @@
       <c r="D41">
         <v>8.61</v>
       </c>
-      <c r="E41">
-        <v>8.61</v>
-      </c>
-      <c r="F41" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C42">
         <v>5</v>
       </c>
       <c r="D42">
-        <v>12.7</v>
-      </c>
-      <c r="E42">
         <v>2.54</v>
       </c>
-      <c r="F42" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B43" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -1640,19 +1510,16 @@
       <c r="D43">
         <v>1.73</v>
       </c>
-      <c r="E43">
-        <v>1.73</v>
-      </c>
-      <c r="F43" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -1660,19 +1527,16 @@
       <c r="D44">
         <v>5.08</v>
       </c>
-      <c r="E44">
-        <v>5.08</v>
-      </c>
-      <c r="F44" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B45" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -1680,19 +1544,16 @@
       <c r="D45">
         <v>0.53500000000000003</v>
       </c>
-      <c r="E45">
-        <v>0.53500000000000003</v>
-      </c>
-      <c r="F45" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -1700,19 +1561,16 @@
       <c r="D46">
         <v>0.36499999999999999</v>
       </c>
-      <c r="E46">
-        <v>0.36499999999999999</v>
-      </c>
-      <c r="F46" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>1607683</v>
       </c>
       <c r="B47" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -1720,11 +1578,8 @@
       <c r="D47">
         <v>0.35299999999999998</v>
       </c>
-      <c r="E47">
-        <v>0.35299999999999998</v>
-      </c>
-      <c r="F47" t="s">
-        <v>97</v>
+      <c r="E47" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Again an update of the partlist
</commit_message>
<xml_diff>
--- a/partlist.xlsx
+++ b/partlist.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
   <si>
     <t>Bestellnr</t>
   </si>
@@ -269,12 +269,6 @@
     <t>http://de.farnell.com/multicomp/bc857a/transistor-pnp-0-1a-45v-sot23/dp/1798068</t>
   </si>
   <si>
-    <t>Prüfbuchse 4mm</t>
-  </si>
-  <si>
-    <t>http://de.farnell.com/hirschmann-testmeasurement/973582101/pr-fbuchse-4mm-pcb-rot-pk5-mls/dp/497332</t>
-  </si>
-  <si>
     <t>Signalrelais IM03TS</t>
   </si>
   <si>
@@ -414,6 +408,24 @@
   </si>
   <si>
     <t>Preis/Stck. [€]</t>
+  </si>
+  <si>
+    <t>Prüfbuchse 4mm, rot</t>
+  </si>
+  <si>
+    <t>PB 4 RT</t>
+  </si>
+  <si>
+    <t>https://www.reichelt.de/Buchsen/PB-4-RT/3/index.html?ACTION=3&amp;GROUPID=5920&amp;ARTICLE=76865&amp;OFFSET=16&amp;</t>
+  </si>
+  <si>
+    <t>https://www.reichelt.de/Buchsen/PB-4-SW/3/index.html?ACTION=3&amp;GROUPID=5626&amp;ARTICLE=13998&amp;OFFSET=16&amp;</t>
+  </si>
+  <si>
+    <t>PB 4 SW</t>
+  </si>
+  <si>
+    <t>Prüfbuchse 4mm, schwarz</t>
   </si>
 </sst>
 </file>
@@ -449,11 +461,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -768,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,7 +794,7 @@
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="100.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="105.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -794,7 +808,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -870,7 +884,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -882,18 +896,18 @@
         <v>0.98</v>
       </c>
       <c r="E6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <v>1.1999999999999999E-3</v>
@@ -921,13 +935,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
       <c r="C9">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D9">
         <v>7.9000000000000008E-3</v>
@@ -938,18 +952,18 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
       </c>
       <c r="C10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -989,7 +1003,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
@@ -1006,7 +1020,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>
@@ -1023,7 +1037,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
         <v>29</v>
@@ -1057,7 +1071,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B17" t="s">
         <v>33</v>
@@ -1074,7 +1088,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B18" t="s">
         <v>35</v>
@@ -1091,7 +1105,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B19" t="s">
         <v>37</v>
@@ -1108,7 +1122,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B20" t="s">
         <v>39</v>
@@ -1119,13 +1133,13 @@
       <c r="D20">
         <v>0.14699999999999999</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B21" t="s">
         <v>41</v>
@@ -1142,7 +1156,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B22" t="s">
         <v>43</v>
@@ -1159,7 +1173,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B23" t="s">
         <v>45</v>
@@ -1193,7 +1207,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B25" t="s">
         <v>49</v>
@@ -1210,7 +1224,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B26" t="s">
         <v>51</v>
@@ -1227,7 +1241,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B27" t="s">
         <v>53</v>
@@ -1244,7 +1258,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B28" t="s">
         <v>55</v>
@@ -1261,7 +1275,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B29" t="s">
         <v>57</v>
@@ -1278,7 +1292,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B30" t="s">
         <v>59</v>
@@ -1295,7 +1309,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B31" t="s">
         <v>61</v>
@@ -1312,7 +1326,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B32" t="s">
         <v>63</v>
@@ -1329,7 +1343,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B33" t="s">
         <v>65</v>
@@ -1346,7 +1360,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B34" t="s">
         <v>67</v>
@@ -1363,7 +1377,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B35" t="s">
         <v>69</v>
@@ -1380,7 +1394,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B36" t="s">
         <v>71</v>
@@ -1397,7 +1411,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B37" t="s">
         <v>73</v>
@@ -1431,7 +1445,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B39" t="s">
         <v>77</v>
@@ -1464,17 +1478,17 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>497332</v>
+      <c r="A41" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="B41" t="s">
         <v>81</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D41">
-        <v>8.61</v>
+        <v>2.54</v>
       </c>
       <c r="E41" t="s">
         <v>82</v>
@@ -1482,16 +1496,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B42" t="s">
         <v>83</v>
       </c>
       <c r="C42">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D42">
-        <v>2.54</v>
+        <v>1.73</v>
       </c>
       <c r="E42" t="s">
         <v>84</v>
@@ -1499,7 +1513,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B43" t="s">
         <v>85</v>
@@ -1508,7 +1522,7 @@
         <v>1</v>
       </c>
       <c r="D43">
-        <v>1.73</v>
+        <v>5.08</v>
       </c>
       <c r="E43" t="s">
         <v>86</v>
@@ -1516,7 +1530,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B44" t="s">
         <v>87</v>
@@ -1525,7 +1539,7 @@
         <v>1</v>
       </c>
       <c r="D44">
-        <v>5.08</v>
+        <v>0.53500000000000003</v>
       </c>
       <c r="E44" t="s">
         <v>88</v>
@@ -1533,7 +1547,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B45" t="s">
         <v>89</v>
@@ -1542,15 +1556,15 @@
         <v>1</v>
       </c>
       <c r="D45">
-        <v>0.53500000000000003</v>
+        <v>0.36499999999999999</v>
       </c>
       <c r="E45" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>127</v>
+      <c r="A46" s="1">
+        <v>1607683</v>
       </c>
       <c r="B46" t="s">
         <v>91</v>
@@ -1559,27 +1573,44 @@
         <v>1</v>
       </c>
       <c r="D46">
-        <v>0.36499999999999999</v>
-      </c>
-      <c r="E46" t="s">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>1607683</v>
+      <c r="A47" t="s">
+        <v>129</v>
       </c>
       <c r="B47" t="s">
-        <v>93</v>
+        <v>128</v>
       </c>
       <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="E47" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>132</v>
+      </c>
+      <c r="B48" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48">
         <v>1</v>
       </c>
-      <c r="D47">
-        <v>0.35299999999999998</v>
-      </c>
-      <c r="E47" t="s">
-        <v>94</v>
+      <c r="D48" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="E48" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>